<commit_message>
new file:   AccessoryOlfactoryBulb/MitralCell/ipython/DelayedRectifierPotassium/.ipynb_checkpoints/iAMC_Kdr-checkpoint.ipynb 	new file:   AccessoryOlfactoryBulb/MitralCell/ipython/DelayedRectifierPotassium/iAMC_Kdr.ipynb 	modified:   AccessoryOlfactoryBulb/MitralCell/ipython/DelayedRectifierPotassium/iAMC_Kdr_kinetics.xlsx 	renamed:    iAMC_NaT.ipynb -> AccessoryOlfactoryBulb/MitralCell/ipython/TransientSodium/iAMC_NaT.ipynb 	renamed:    iAMC_kinetics.xlsx -> AccessoryOlfactoryBulb/MitralCell/ipython/TransientSodium/iAMC_kinetics.xlsx
</commit_message>
<xml_diff>
--- a/AccessoryOlfactoryBulb/MitralCell/ipython/DelayedRectifierPotassium/iAMC_Kdr_kinetics.xlsx
+++ b/AccessoryOlfactoryBulb/MitralCell/ipython/DelayedRectifierPotassium/iAMC_Kdr_kinetics.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Kdr_amp" sheetId="1" r:id="rId1"/>
@@ -16,18 +16,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="1">
   <si>
-    <t>Vmem (mV)</t>
-  </si>
-  <si>
-    <t>Kdr_amplitude (pA/pF)</t>
-  </si>
-  <si>
-    <t>Kdr_tau_activation (ms)</t>
-  </si>
-  <si>
-    <t>Kdr_tau_deactivation (ms)</t>
+    <t>mean</t>
   </si>
 </sst>
 </file>
@@ -52,10 +43,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <u/>
       <sz val="11"/>
-      <color rgb="FFC00000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -388,8 +376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AP2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:AP2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -398,9 +386,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:42">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="A1" s="1"/>
       <c r="B1" s="2">
         <v>-100</v>
       </c>
@@ -527,7 +513,7 @@
     </row>
     <row r="2" spans="1:42">
       <c r="A2" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
@@ -655,6 +641,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -663,7 +650,7 @@
   <dimension ref="A1:W2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:W2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -672,9 +659,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="A1" s="1"/>
       <c r="B1" s="2">
         <v>-55</v>
       </c>
@@ -744,7 +729,7 @@
     </row>
     <row r="2" spans="1:23">
       <c r="A2" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2">
         <v>47.598666666666666</v>
@@ -822,8 +807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:W2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -832,9 +817,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="A1" s="1"/>
       <c r="B1" s="2">
         <v>-55</v>
       </c>
@@ -904,7 +887,7 @@
     </row>
     <row r="2" spans="1:23">
       <c r="A2" s="3" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2">
         <v>43.225749999999998</v>

</xml_diff>